<commit_message>
add analyse detail and reform macro class
</commit_message>
<xml_diff>
--- a/database/industries/dode/shekarbon/balancesheet/yearly.xlsx
+++ b/database/industries/dode/shekarbon/balancesheet/yearly.xlsx
@@ -192,6 +192,11 @@
     <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
+    <col min="10" max="10" width="29" customWidth="1"/>
+    <col min="11" max="11" width="29" customWidth="1"/>
+    <col min="12" max="12" width="29" customWidth="1"/>
+    <col min="13" max="13" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -216,6 +221,21 @@
       <c r="H1" s="2">
         <v/>
       </c>
+      <c r="I1" s="2">
+        <v/>
+      </c>
+      <c r="J1" s="2">
+        <v/>
+      </c>
+      <c r="K1" s="2">
+        <v/>
+      </c>
+      <c r="L1" s="2">
+        <v/>
+      </c>
+      <c r="M1" s="2">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="3" t="inlineStr">
@@ -241,6 +261,21 @@
       <c r="H2" s="2">
         <v/>
       </c>
+      <c r="I2" s="2">
+        <v/>
+      </c>
+      <c r="J2" s="2">
+        <v/>
+      </c>
+      <c r="K2" s="2">
+        <v/>
+      </c>
+      <c r="L2" s="2">
+        <v/>
+      </c>
+      <c r="M2" s="2">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="4" t="inlineStr">
@@ -266,6 +301,21 @@
       <c r="H3" s="2">
         <v/>
       </c>
+      <c r="I3" s="2">
+        <v/>
+      </c>
+      <c r="J3" s="2">
+        <v/>
+      </c>
+      <c r="K3" s="2">
+        <v/>
+      </c>
+      <c r="L3" s="2">
+        <v/>
+      </c>
+      <c r="M3" s="2">
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="2">
@@ -289,6 +339,21 @@
       <c r="H4" s="2">
         <v/>
       </c>
+      <c r="I4" s="2">
+        <v/>
+      </c>
+      <c r="J4" s="2">
+        <v/>
+      </c>
+      <c r="K4" s="2">
+        <v/>
+      </c>
+      <c r="L4" s="2">
+        <v/>
+      </c>
+      <c r="M4" s="2">
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="5" t="inlineStr">
@@ -314,6 +379,21 @@
       <c r="H5" s="5">
         <v/>
       </c>
+      <c r="I5" s="5">
+        <v/>
+      </c>
+      <c r="J5" s="5">
+        <v/>
+      </c>
+      <c r="K5" s="5">
+        <v/>
+      </c>
+      <c r="L5" s="5">
+        <v/>
+      </c>
+      <c r="M5" s="5">
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="6" t="inlineStr">
@@ -339,6 +419,21 @@
       <c r="H6" s="5">
         <v/>
       </c>
+      <c r="I6" s="5">
+        <v/>
+      </c>
+      <c r="J6" s="5">
+        <v/>
+      </c>
+      <c r="K6" s="5">
+        <v/>
+      </c>
+      <c r="L6" s="5">
+        <v/>
+      </c>
+      <c r="M6" s="5">
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="2">
@@ -362,6 +457,21 @@
       <c r="H7" s="2">
         <v/>
       </c>
+      <c r="I7" s="2">
+        <v/>
+      </c>
+      <c r="J7" s="2">
+        <v/>
+      </c>
+      <c r="K7" s="2">
+        <v/>
+      </c>
+      <c r="L7" s="2">
+        <v/>
+      </c>
+      <c r="M7" s="2">
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="8" t="inlineStr">
@@ -374,25 +484,50 @@
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
+          <t>12 ماهه منتهی به 1391/12</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1392/12</t>
+        </is>
+      </c>
+      <c r="F8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1393/12</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1394/12</t>
+        </is>
+      </c>
+      <c r="H8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1395/12</t>
+        </is>
+      </c>
+      <c r="I8" s="7" t="inlineStr">
+        <is>
           <t>12 ماهه منتهی به 1396/12</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr">
+      <c r="J8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1397/12</t>
         </is>
       </c>
-      <c r="F8" s="7" t="inlineStr">
+      <c r="K8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1398/12</t>
         </is>
       </c>
-      <c r="G8" s="7" t="inlineStr">
+      <c r="L8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1399/12</t>
         </is>
       </c>
-      <c r="H8" s="7" t="inlineStr">
+      <c r="M8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1400/12</t>
         </is>
@@ -409,27 +544,52 @@
       </c>
       <c r="D9" s="10" t="inlineStr">
         <is>
+          <t>1393-04-19 (7)</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="inlineStr">
+        <is>
+          <t>1394-03-07 (7)</t>
+        </is>
+      </c>
+      <c r="F9" s="10" t="inlineStr">
+        <is>
+          <t>1395-03-19 (7)</t>
+        </is>
+      </c>
+      <c r="G9" s="10" t="inlineStr">
+        <is>
+          <t>1396-03-09 (8)</t>
+        </is>
+      </c>
+      <c r="H9" s="10" t="inlineStr">
+        <is>
+          <t>1397-03-10 (9)</t>
+        </is>
+      </c>
+      <c r="I9" s="10" t="inlineStr">
+        <is>
           <t>1398-03-09 (8)</t>
         </is>
       </c>
-      <c r="E9" s="10" t="inlineStr">
+      <c r="J9" s="10" t="inlineStr">
         <is>
           <t>1399-03-09 (8)</t>
         </is>
       </c>
-      <c r="F9" s="10" t="inlineStr">
+      <c r="K9" s="10" t="inlineStr">
         <is>
           <t>1400-03-10 (9)</t>
         </is>
       </c>
-      <c r="G9" s="10" t="inlineStr">
+      <c r="L9" s="10" t="inlineStr">
         <is>
           <t>1401-03-09 (9)</t>
         </is>
       </c>
-      <c r="H9" s="10" t="inlineStr">
-        <is>
-          <t>1401-04-30 (3)</t>
+      <c r="M9" s="10" t="inlineStr">
+        <is>
+          <t>1401-07-30 (4)</t>
         </is>
       </c>
     </row>
@@ -455,6 +615,21 @@
       <c r="H10" s="12">
         <v/>
       </c>
+      <c r="I10" s="12">
+        <v/>
+      </c>
+      <c r="J10" s="12">
+        <v/>
+      </c>
+      <c r="K10" s="12">
+        <v/>
+      </c>
+      <c r="L10" s="12">
+        <v/>
+      </c>
+      <c r="M10" s="12">
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -480,6 +655,21 @@
       <c r="H11" s="14">
         <v/>
       </c>
+      <c r="I11" s="14">
+        <v/>
+      </c>
+      <c r="J11" s="14">
+        <v/>
+      </c>
+      <c r="K11" s="14">
+        <v/>
+      </c>
+      <c r="L11" s="14">
+        <v/>
+      </c>
+      <c r="M11" s="14">
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="15" t="inlineStr">
@@ -491,18 +681,33 @@
         <v/>
       </c>
       <c r="D12" s="16">
+        <v>22313</v>
+      </c>
+      <c r="E12" s="16">
+        <v>16358</v>
+      </c>
+      <c r="F12" s="16">
+        <v>9091</v>
+      </c>
+      <c r="G12" s="16">
+        <v>30293</v>
+      </c>
+      <c r="H12" s="16">
+        <v>14658</v>
+      </c>
+      <c r="I12" s="16">
         <v>65218</v>
       </c>
-      <c r="E12" s="16">
+      <c r="J12" s="16">
         <v>92009</v>
       </c>
-      <c r="F12" s="16">
+      <c r="K12" s="16">
         <v>65100</v>
       </c>
-      <c r="G12" s="16">
+      <c r="L12" s="16">
         <v>271614</v>
       </c>
-      <c r="H12" s="16">
+      <c r="M12" s="16">
         <v>474356</v>
       </c>
     </row>
@@ -516,18 +721,33 @@
         <v/>
       </c>
       <c r="D13" s="12">
+        <v>1665</v>
+      </c>
+      <c r="E13" s="12">
+        <v>4043</v>
+      </c>
+      <c r="F13" s="12">
+        <v>3597</v>
+      </c>
+      <c r="G13" s="12">
+        <v>4650</v>
+      </c>
+      <c r="H13" s="12">
+        <v>4825</v>
+      </c>
+      <c r="I13" s="12">
         <v>5519</v>
       </c>
-      <c r="E13" s="12">
+      <c r="J13" s="12">
         <v>8034</v>
       </c>
-      <c r="F13" s="12">
+      <c r="K13" s="12">
         <v>8532</v>
       </c>
-      <c r="G13" s="12">
+      <c r="L13" s="12">
         <v>2972</v>
       </c>
-      <c r="H13" s="12">
+      <c r="M13" s="12">
         <v>2972</v>
       </c>
     </row>
@@ -541,18 +761,33 @@
         <v/>
       </c>
       <c r="D14" s="16">
+        <v>376822</v>
+      </c>
+      <c r="E14" s="16">
+        <v>446028</v>
+      </c>
+      <c r="F14" s="16">
+        <v>518811</v>
+      </c>
+      <c r="G14" s="16">
+        <v>603585</v>
+      </c>
+      <c r="H14" s="16">
+        <v>617580</v>
+      </c>
+      <c r="I14" s="16">
         <v>652635</v>
       </c>
-      <c r="E14" s="16">
+      <c r="J14" s="16">
         <v>440800</v>
       </c>
-      <c r="F14" s="16">
+      <c r="K14" s="16">
         <v>694513</v>
       </c>
-      <c r="G14" s="16">
+      <c r="L14" s="16">
         <v>1006407</v>
       </c>
-      <c r="H14" s="16">
+      <c r="M14" s="16">
         <v>2622056</v>
       </c>
     </row>
@@ -566,18 +801,33 @@
         <v/>
       </c>
       <c r="D15" s="12">
+        <v>155872</v>
+      </c>
+      <c r="E15" s="12">
+        <v>248871</v>
+      </c>
+      <c r="F15" s="12">
+        <v>249323</v>
+      </c>
+      <c r="G15" s="12">
+        <v>126217</v>
+      </c>
+      <c r="H15" s="12">
+        <v>206507</v>
+      </c>
+      <c r="I15" s="12">
         <v>317101</v>
       </c>
-      <c r="E15" s="12">
+      <c r="J15" s="12">
         <v>483343</v>
       </c>
-      <c r="F15" s="12">
+      <c r="K15" s="12">
         <v>653067</v>
       </c>
-      <c r="G15" s="12">
+      <c r="L15" s="12">
         <v>925246</v>
       </c>
-      <c r="H15" s="12">
+      <c r="M15" s="12">
         <v>1818618</v>
       </c>
     </row>
@@ -591,18 +841,33 @@
         <v/>
       </c>
       <c r="D16" s="16">
+        <v>83906</v>
+      </c>
+      <c r="E16" s="16">
+        <v>17087</v>
+      </c>
+      <c r="F16" s="16">
+        <v>13099</v>
+      </c>
+      <c r="G16" s="16">
+        <v>10964</v>
+      </c>
+      <c r="H16" s="16">
+        <v>11745</v>
+      </c>
+      <c r="I16" s="16">
         <v>56466</v>
       </c>
-      <c r="E16" s="16">
+      <c r="J16" s="16">
         <v>371476</v>
       </c>
-      <c r="F16" s="16">
+      <c r="K16" s="16">
         <v>125529</v>
       </c>
-      <c r="G16" s="16">
+      <c r="L16" s="16">
         <v>841628</v>
       </c>
-      <c r="H16" s="16">
+      <c r="M16" s="16">
         <v>614746</v>
       </c>
     </row>
@@ -616,18 +881,33 @@
         <v/>
       </c>
       <c r="D17" s="12">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
         <v>144515</v>
       </c>
-      <c r="E17" s="12">
+      <c r="J17" s="12">
         <v>144515</v>
       </c>
-      <c r="F17" s="12">
-        <v>0</v>
-      </c>
-      <c r="G17" s="12">
-        <v>0</v>
-      </c>
-      <c r="H17" s="12">
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
+        <v>0</v>
+      </c>
+      <c r="M17" s="12">
         <v>0</v>
       </c>
     </row>
@@ -641,18 +921,33 @@
         <v/>
       </c>
       <c r="D18" s="18">
+        <v>640578</v>
+      </c>
+      <c r="E18" s="18">
+        <v>732387</v>
+      </c>
+      <c r="F18" s="18">
+        <v>793921</v>
+      </c>
+      <c r="G18" s="18">
+        <v>775709</v>
+      </c>
+      <c r="H18" s="18">
+        <v>855315</v>
+      </c>
+      <c r="I18" s="18">
         <v>1241454</v>
       </c>
-      <c r="E18" s="18">
+      <c r="J18" s="18">
         <v>1540177</v>
       </c>
-      <c r="F18" s="18">
+      <c r="K18" s="18">
         <v>1546741</v>
       </c>
-      <c r="G18" s="18">
+      <c r="L18" s="18">
         <v>3047867</v>
       </c>
-      <c r="H18" s="18">
+      <c r="M18" s="18">
         <v>5532748</v>
       </c>
     </row>
@@ -680,6 +975,21 @@
       <c r="H19" s="12">
         <v>0</v>
       </c>
+      <c r="I19" s="12">
+        <v>0</v>
+      </c>
+      <c r="J19" s="12">
+        <v>0</v>
+      </c>
+      <c r="K19" s="12">
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
+        <v>0</v>
+      </c>
+      <c r="M19" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="15" t="inlineStr">
@@ -691,18 +1001,33 @@
         <v/>
       </c>
       <c r="D20" s="16">
+        <v>372125</v>
+      </c>
+      <c r="E20" s="16">
+        <v>385484</v>
+      </c>
+      <c r="F20" s="16">
+        <v>385484</v>
+      </c>
+      <c r="G20" s="16">
+        <v>385484</v>
+      </c>
+      <c r="H20" s="16">
+        <v>413845</v>
+      </c>
+      <c r="I20" s="16">
         <v>269330</v>
       </c>
-      <c r="E20" s="16">
+      <c r="J20" s="16">
         <v>269332</v>
       </c>
-      <c r="F20" s="16">
+      <c r="K20" s="16">
         <v>413823</v>
       </c>
-      <c r="G20" s="16">
+      <c r="L20" s="16">
         <v>659525</v>
       </c>
-      <c r="H20" s="16">
+      <c r="M20" s="16">
         <v>869459</v>
       </c>
     </row>
@@ -715,11 +1040,15 @@
       <c r="C21" s="12">
         <v/>
       </c>
-      <c r="D21" s="12">
-        <v>0</v>
-      </c>
-      <c r="E21" s="12">
-        <v>0</v>
+      <c r="D21" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F21" s="12">
         <v>0</v>
@@ -728,6 +1057,21 @@
         <v>0</v>
       </c>
       <c r="H21" s="12">
+        <v>0</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0</v>
+      </c>
+      <c r="K21" s="12">
+        <v>0</v>
+      </c>
+      <c r="L21" s="12">
+        <v>0</v>
+      </c>
+      <c r="M21" s="12">
         <v>0</v>
       </c>
     </row>
@@ -741,18 +1085,33 @@
         <v/>
       </c>
       <c r="D22" s="16">
+        <v>81532</v>
+      </c>
+      <c r="E22" s="16">
+        <v>135133</v>
+      </c>
+      <c r="F22" s="16">
+        <v>145809</v>
+      </c>
+      <c r="G22" s="16">
+        <v>144365</v>
+      </c>
+      <c r="H22" s="16">
+        <v>141450</v>
+      </c>
+      <c r="I22" s="16">
         <v>157529</v>
       </c>
-      <c r="E22" s="16">
+      <c r="J22" s="16">
         <v>220004</v>
       </c>
-      <c r="F22" s="16">
+      <c r="K22" s="16">
         <v>283486</v>
       </c>
-      <c r="G22" s="16">
+      <c r="L22" s="16">
         <v>282504</v>
       </c>
-      <c r="H22" s="16">
+      <c r="M22" s="16">
         <v>6532795</v>
       </c>
     </row>
@@ -766,18 +1125,33 @@
         <v/>
       </c>
       <c r="D23" s="12">
+        <v>2218</v>
+      </c>
+      <c r="E23" s="12">
+        <v>2112</v>
+      </c>
+      <c r="F23" s="12">
+        <v>2048</v>
+      </c>
+      <c r="G23" s="12">
+        <v>2091</v>
+      </c>
+      <c r="H23" s="12">
+        <v>2005</v>
+      </c>
+      <c r="I23" s="12">
         <v>1940</v>
       </c>
-      <c r="E23" s="12">
+      <c r="J23" s="12">
         <v>23618</v>
       </c>
-      <c r="F23" s="12">
+      <c r="K23" s="12">
         <v>25093</v>
       </c>
-      <c r="G23" s="12">
+      <c r="L23" s="12">
         <v>25586</v>
       </c>
-      <c r="H23" s="12">
+      <c r="M23" s="12">
         <v>23812</v>
       </c>
     </row>
@@ -790,15 +1164,11 @@
       <c r="C24" s="16">
         <v/>
       </c>
-      <c r="D24" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E24" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D24" s="16">
+        <v>0</v>
+      </c>
+      <c r="E24" s="16">
+        <v>0</v>
       </c>
       <c r="F24" s="16" t="inlineStr">
         <is>
@@ -811,6 +1181,31 @@
         </is>
       </c>
       <c r="H24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M24" s="16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -840,6 +1235,21 @@
       <c r="H25" s="12">
         <v>0</v>
       </c>
+      <c r="I25" s="12">
+        <v>0</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0</v>
+      </c>
+      <c r="K25" s="12">
+        <v>0</v>
+      </c>
+      <c r="L25" s="12">
+        <v>0</v>
+      </c>
+      <c r="M25" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="17" t="inlineStr">
@@ -851,18 +1261,33 @@
         <v/>
       </c>
       <c r="D26" s="18">
+        <v>455875</v>
+      </c>
+      <c r="E26" s="18">
+        <v>522729</v>
+      </c>
+      <c r="F26" s="18">
+        <v>533341</v>
+      </c>
+      <c r="G26" s="18">
+        <v>531940</v>
+      </c>
+      <c r="H26" s="18">
+        <v>557300</v>
+      </c>
+      <c r="I26" s="18">
         <v>428799</v>
       </c>
-      <c r="E26" s="18">
+      <c r="J26" s="18">
         <v>512954</v>
       </c>
-      <c r="F26" s="18">
+      <c r="K26" s="18">
         <v>722402</v>
       </c>
-      <c r="G26" s="18">
+      <c r="L26" s="18">
         <v>967615</v>
       </c>
-      <c r="H26" s="18">
+      <c r="M26" s="18">
         <v>7426066</v>
       </c>
     </row>
@@ -876,18 +1301,33 @@
         <v/>
       </c>
       <c r="D27" s="20">
+        <v>1096453</v>
+      </c>
+      <c r="E27" s="20">
+        <v>1255116</v>
+      </c>
+      <c r="F27" s="20">
+        <v>1327262</v>
+      </c>
+      <c r="G27" s="20">
+        <v>1307649</v>
+      </c>
+      <c r="H27" s="20">
+        <v>1412615</v>
+      </c>
+      <c r="I27" s="20">
         <v>1670253</v>
       </c>
-      <c r="E27" s="20">
+      <c r="J27" s="20">
         <v>2053131</v>
       </c>
-      <c r="F27" s="20">
+      <c r="K27" s="20">
         <v>2269143</v>
       </c>
-      <c r="G27" s="20">
+      <c r="L27" s="20">
         <v>4015482</v>
       </c>
-      <c r="H27" s="20">
+      <c r="M27" s="20">
         <v>12958814</v>
       </c>
     </row>
@@ -915,6 +1355,21 @@
       <c r="H28" s="14">
         <v/>
       </c>
+      <c r="I28" s="14">
+        <v/>
+      </c>
+      <c r="J28" s="14">
+        <v/>
+      </c>
+      <c r="K28" s="14">
+        <v/>
+      </c>
+      <c r="L28" s="14">
+        <v/>
+      </c>
+      <c r="M28" s="14">
+        <v/>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="15" t="inlineStr">
@@ -926,18 +1381,33 @@
         <v/>
       </c>
       <c r="D29" s="16">
+        <v>274512</v>
+      </c>
+      <c r="E29" s="16">
+        <v>365010</v>
+      </c>
+      <c r="F29" s="16">
+        <v>459940</v>
+      </c>
+      <c r="G29" s="16">
+        <v>463120</v>
+      </c>
+      <c r="H29" s="16">
+        <v>553524</v>
+      </c>
+      <c r="I29" s="16">
         <v>492667</v>
       </c>
-      <c r="E29" s="16">
+      <c r="J29" s="16">
         <v>494547</v>
       </c>
-      <c r="F29" s="16">
+      <c r="K29" s="16">
         <v>417434</v>
       </c>
-      <c r="G29" s="16">
+      <c r="L29" s="16">
         <v>907752</v>
       </c>
-      <c r="H29" s="16">
+      <c r="M29" s="16">
         <v>1323644</v>
       </c>
     </row>
@@ -950,15 +1420,11 @@
       <c r="C30" s="12">
         <v/>
       </c>
-      <c r="D30" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E30" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D30" s="12">
+        <v>0</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0</v>
       </c>
       <c r="F30" s="12" t="inlineStr">
         <is>
@@ -971,6 +1437,31 @@
         </is>
       </c>
       <c r="H30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M30" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -986,18 +1477,33 @@
         <v/>
       </c>
       <c r="D31" s="16">
+        <v>22565</v>
+      </c>
+      <c r="E31" s="16">
+        <v>10089</v>
+      </c>
+      <c r="F31" s="16">
+        <v>28797</v>
+      </c>
+      <c r="G31" s="16">
+        <v>3302</v>
+      </c>
+      <c r="H31" s="16">
+        <v>6872</v>
+      </c>
+      <c r="I31" s="16">
         <v>59867</v>
       </c>
-      <c r="E31" s="16">
+      <c r="J31" s="16">
         <v>104557</v>
       </c>
-      <c r="F31" s="16">
+      <c r="K31" s="16">
         <v>110496</v>
       </c>
-      <c r="G31" s="16">
+      <c r="L31" s="16">
         <v>505827</v>
       </c>
-      <c r="H31" s="16">
+      <c r="M31" s="16">
         <v>440510</v>
       </c>
     </row>
@@ -1011,18 +1517,33 @@
         <v/>
       </c>
       <c r="D32" s="12">
+        <v>25751</v>
+      </c>
+      <c r="E32" s="12">
+        <v>48704</v>
+      </c>
+      <c r="F32" s="12">
+        <v>27839</v>
+      </c>
+      <c r="G32" s="12">
+        <v>36720</v>
+      </c>
+      <c r="H32" s="12">
+        <v>42255</v>
+      </c>
+      <c r="I32" s="12">
         <v>83196</v>
       </c>
-      <c r="E32" s="12">
+      <c r="J32" s="12">
         <v>169434</v>
       </c>
-      <c r="F32" s="12">
+      <c r="K32" s="12">
         <v>166402</v>
       </c>
-      <c r="G32" s="12">
+      <c r="L32" s="12">
         <v>212925</v>
       </c>
-      <c r="H32" s="12">
+      <c r="M32" s="12">
         <v>324504</v>
       </c>
     </row>
@@ -1036,18 +1557,33 @@
         <v/>
       </c>
       <c r="D33" s="16">
+        <v>37595</v>
+      </c>
+      <c r="E33" s="16">
+        <v>16662</v>
+      </c>
+      <c r="F33" s="16">
+        <v>68984</v>
+      </c>
+      <c r="G33" s="16">
+        <v>91742</v>
+      </c>
+      <c r="H33" s="16">
+        <v>97418</v>
+      </c>
+      <c r="I33" s="16">
         <v>83155</v>
       </c>
-      <c r="E33" s="16">
+      <c r="J33" s="16">
         <v>73321</v>
       </c>
-      <c r="F33" s="16">
+      <c r="K33" s="16">
         <v>83479</v>
       </c>
-      <c r="G33" s="16">
+      <c r="L33" s="16">
         <v>127465</v>
       </c>
-      <c r="H33" s="16">
+      <c r="M33" s="16">
         <v>616769</v>
       </c>
     </row>
@@ -1061,18 +1597,33 @@
         <v/>
       </c>
       <c r="D34" s="12">
+        <v>162729</v>
+      </c>
+      <c r="E34" s="12">
+        <v>203791</v>
+      </c>
+      <c r="F34" s="12">
+        <v>119155</v>
+      </c>
+      <c r="G34" s="12">
+        <v>118374</v>
+      </c>
+      <c r="H34" s="12">
+        <v>127332</v>
+      </c>
+      <c r="I34" s="12">
         <v>138146</v>
       </c>
-      <c r="E34" s="12">
+      <c r="J34" s="12">
         <v>99862</v>
       </c>
-      <c r="F34" s="12">
+      <c r="K34" s="12">
         <v>177043</v>
       </c>
-      <c r="G34" s="12">
+      <c r="L34" s="12">
         <v>185826</v>
       </c>
-      <c r="H34" s="12">
+      <c r="M34" s="12">
         <v>327717</v>
       </c>
     </row>
@@ -1085,11 +1636,15 @@
       <c r="C35" s="16">
         <v/>
       </c>
-      <c r="D35" s="16">
-        <v>0</v>
-      </c>
-      <c r="E35" s="16">
-        <v>0</v>
+      <c r="D35" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F35" s="16">
         <v>0</v>
@@ -1098,6 +1653,21 @@
         <v>0</v>
       </c>
       <c r="H35" s="16">
+        <v>0</v>
+      </c>
+      <c r="I35" s="16">
+        <v>0</v>
+      </c>
+      <c r="J35" s="16">
+        <v>0</v>
+      </c>
+      <c r="K35" s="16">
+        <v>0</v>
+      </c>
+      <c r="L35" s="16">
+        <v>0</v>
+      </c>
+      <c r="M35" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1125,6 +1695,21 @@
       <c r="H36" s="12">
         <v>0</v>
       </c>
+      <c r="I36" s="12">
+        <v>0</v>
+      </c>
+      <c r="J36" s="12">
+        <v>0</v>
+      </c>
+      <c r="K36" s="12">
+        <v>0</v>
+      </c>
+      <c r="L36" s="12">
+        <v>0</v>
+      </c>
+      <c r="M36" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="17" t="inlineStr">
@@ -1136,18 +1721,33 @@
         <v/>
       </c>
       <c r="D37" s="18">
+        <v>523152</v>
+      </c>
+      <c r="E37" s="18">
+        <v>644256</v>
+      </c>
+      <c r="F37" s="18">
+        <v>704715</v>
+      </c>
+      <c r="G37" s="18">
+        <v>713258</v>
+      </c>
+      <c r="H37" s="18">
+        <v>827401</v>
+      </c>
+      <c r="I37" s="18">
         <v>857031</v>
       </c>
-      <c r="E37" s="18">
+      <c r="J37" s="18">
         <v>941721</v>
       </c>
-      <c r="F37" s="18">
+      <c r="K37" s="18">
         <v>954854</v>
       </c>
-      <c r="G37" s="18">
+      <c r="L37" s="18">
         <v>1939795</v>
       </c>
-      <c r="H37" s="18">
+      <c r="M37" s="18">
         <v>3033144</v>
       </c>
     </row>
@@ -1161,18 +1761,33 @@
         <v/>
       </c>
       <c r="D38" s="12">
-        <v>0</v>
+        <v>8431</v>
       </c>
       <c r="E38" s="12">
         <v>0</v>
       </c>
       <c r="F38" s="12">
+        <v>0</v>
+      </c>
+      <c r="G38" s="12">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0</v>
+      </c>
+      <c r="I38" s="12">
+        <v>0</v>
+      </c>
+      <c r="J38" s="12">
+        <v>0</v>
+      </c>
+      <c r="K38" s="12">
         <v>462075</v>
       </c>
-      <c r="G38" s="12">
+      <c r="L38" s="12">
         <v>662279</v>
       </c>
-      <c r="H38" s="12">
+      <c r="M38" s="12">
         <v>861203</v>
       </c>
     </row>
@@ -1185,25 +1800,44 @@
       <c r="C39" s="16">
         <v/>
       </c>
-      <c r="D39" s="16">
-        <v>0</v>
+      <c r="D39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="E39" s="16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F39" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G39" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H39" s="16" t="inlineStr">
+      <c r="F39" s="16">
+        <v>0</v>
+      </c>
+      <c r="G39" s="16">
+        <v>0</v>
+      </c>
+      <c r="H39" s="16">
+        <v>0</v>
+      </c>
+      <c r="I39" s="16">
+        <v>0</v>
+      </c>
+      <c r="J39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M39" s="16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1219,18 +1853,33 @@
         <v/>
       </c>
       <c r="D40" s="12">
-        <v>0</v>
+        <v>125791</v>
       </c>
       <c r="E40" s="12">
-        <v>0</v>
+        <v>11539</v>
       </c>
       <c r="F40" s="12">
-        <v>0</v>
+        <v>33239</v>
       </c>
       <c r="G40" s="12">
-        <v>0</v>
+        <v>6298</v>
       </c>
       <c r="H40" s="12">
+        <v>0</v>
+      </c>
+      <c r="I40" s="12">
+        <v>0</v>
+      </c>
+      <c r="J40" s="12">
+        <v>0</v>
+      </c>
+      <c r="K40" s="12">
+        <v>0</v>
+      </c>
+      <c r="L40" s="12">
+        <v>0</v>
+      </c>
+      <c r="M40" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1244,18 +1893,33 @@
         <v/>
       </c>
       <c r="D41" s="16">
+        <v>20035</v>
+      </c>
+      <c r="E41" s="16">
+        <v>21770</v>
+      </c>
+      <c r="F41" s="16">
+        <v>22389</v>
+      </c>
+      <c r="G41" s="16">
+        <v>27196</v>
+      </c>
+      <c r="H41" s="16">
+        <v>27598</v>
+      </c>
+      <c r="I41" s="16">
         <v>24583</v>
       </c>
-      <c r="E41" s="16">
+      <c r="J41" s="16">
         <v>23667</v>
       </c>
-      <c r="F41" s="16">
+      <c r="K41" s="16">
         <v>32582</v>
       </c>
-      <c r="G41" s="16">
+      <c r="L41" s="16">
         <v>40090</v>
       </c>
-      <c r="H41" s="16">
+      <c r="M41" s="16">
         <v>52936</v>
       </c>
     </row>
@@ -1269,18 +1933,33 @@
         <v/>
       </c>
       <c r="D42" s="20">
+        <v>154257</v>
+      </c>
+      <c r="E42" s="20">
+        <v>33309</v>
+      </c>
+      <c r="F42" s="20">
+        <v>55628</v>
+      </c>
+      <c r="G42" s="20">
+        <v>33494</v>
+      </c>
+      <c r="H42" s="20">
+        <v>27598</v>
+      </c>
+      <c r="I42" s="20">
         <v>24583</v>
       </c>
-      <c r="E42" s="20">
+      <c r="J42" s="20">
         <v>23667</v>
       </c>
-      <c r="F42" s="20">
+      <c r="K42" s="20">
         <v>494657</v>
       </c>
-      <c r="G42" s="20">
+      <c r="L42" s="20">
         <v>702369</v>
       </c>
-      <c r="H42" s="20">
+      <c r="M42" s="20">
         <v>914139</v>
       </c>
     </row>
@@ -1294,18 +1973,33 @@
         <v/>
       </c>
       <c r="D43" s="18">
+        <v>677409</v>
+      </c>
+      <c r="E43" s="18">
+        <v>677565</v>
+      </c>
+      <c r="F43" s="18">
+        <v>760343</v>
+      </c>
+      <c r="G43" s="18">
+        <v>746752</v>
+      </c>
+      <c r="H43" s="18">
+        <v>854999</v>
+      </c>
+      <c r="I43" s="18">
         <v>881614</v>
       </c>
-      <c r="E43" s="18">
+      <c r="J43" s="18">
         <v>965388</v>
       </c>
-      <c r="F43" s="18">
+      <c r="K43" s="18">
         <v>1449511</v>
       </c>
-      <c r="G43" s="18">
+      <c r="L43" s="18">
         <v>2642164</v>
       </c>
-      <c r="H43" s="18">
+      <c r="M43" s="18">
         <v>3947283</v>
       </c>
     </row>
@@ -1333,6 +2027,21 @@
       <c r="H44" s="14">
         <v/>
       </c>
+      <c r="I44" s="14">
+        <v/>
+      </c>
+      <c r="J44" s="14">
+        <v/>
+      </c>
+      <c r="K44" s="14">
+        <v/>
+      </c>
+      <c r="L44" s="14">
+        <v/>
+      </c>
+      <c r="M44" s="14">
+        <v/>
+      </c>
     </row>
     <row r="45">
       <c r="B45" s="15" t="inlineStr">
@@ -1356,6 +2065,21 @@
         <v>250000</v>
       </c>
       <c r="H45" s="16">
+        <v>250000</v>
+      </c>
+      <c r="I45" s="16">
+        <v>250000</v>
+      </c>
+      <c r="J45" s="16">
+        <v>250000</v>
+      </c>
+      <c r="K45" s="16">
+        <v>250000</v>
+      </c>
+      <c r="L45" s="16">
+        <v>250000</v>
+      </c>
+      <c r="M45" s="16">
         <v>6385128</v>
       </c>
     </row>
@@ -1383,6 +2107,21 @@
       <c r="H46" s="12">
         <v>0</v>
       </c>
+      <c r="I46" s="12">
+        <v>0</v>
+      </c>
+      <c r="J46" s="12">
+        <v>0</v>
+      </c>
+      <c r="K46" s="12">
+        <v>0</v>
+      </c>
+      <c r="L46" s="12">
+        <v>0</v>
+      </c>
+      <c r="M46" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" s="15" t="inlineStr">
@@ -1408,6 +2147,21 @@
       <c r="H47" s="16">
         <v>0</v>
       </c>
+      <c r="I47" s="16">
+        <v>0</v>
+      </c>
+      <c r="J47" s="16">
+        <v>0</v>
+      </c>
+      <c r="K47" s="16">
+        <v>0</v>
+      </c>
+      <c r="L47" s="16">
+        <v>0</v>
+      </c>
+      <c r="M47" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="B48" s="11" t="inlineStr">
@@ -1418,19 +2172,38 @@
       <c r="C48" s="12">
         <v/>
       </c>
-      <c r="D48" s="12">
-        <v>0</v>
-      </c>
-      <c r="E48" s="12">
-        <v>0</v>
+      <c r="D48" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E48" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F48" s="12">
         <v>0</v>
       </c>
       <c r="G48" s="12">
+        <v>0</v>
+      </c>
+      <c r="H48" s="12">
+        <v>0</v>
+      </c>
+      <c r="I48" s="12">
+        <v>0</v>
+      </c>
+      <c r="J48" s="12">
+        <v>0</v>
+      </c>
+      <c r="K48" s="12">
+        <v>0</v>
+      </c>
+      <c r="L48" s="12">
         <v>-233358</v>
       </c>
-      <c r="H48" s="12">
+      <c r="M48" s="12">
         <v>-344777</v>
       </c>
     </row>
@@ -1448,16 +2221,41 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E49" s="16">
-        <v>0</v>
-      </c>
-      <c r="F49" s="16">
-        <v>0</v>
-      </c>
-      <c r="G49" s="16">
-        <v>0</v>
-      </c>
-      <c r="H49" s="16">
+      <c r="E49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J49" s="16">
+        <v>0</v>
+      </c>
+      <c r="K49" s="16">
+        <v>0</v>
+      </c>
+      <c r="L49" s="16">
+        <v>0</v>
+      </c>
+      <c r="M49" s="16">
         <v>19064</v>
       </c>
     </row>
@@ -1485,6 +2283,21 @@
       <c r="H50" s="12">
         <v>25000</v>
       </c>
+      <c r="I50" s="12">
+        <v>25000</v>
+      </c>
+      <c r="J50" s="12">
+        <v>25000</v>
+      </c>
+      <c r="K50" s="12">
+        <v>25000</v>
+      </c>
+      <c r="L50" s="12">
+        <v>25000</v>
+      </c>
+      <c r="M50" s="12">
+        <v>25000</v>
+      </c>
     </row>
     <row r="51">
       <c r="B51" s="15" t="inlineStr">
@@ -1510,6 +2323,21 @@
       <c r="H51" s="16">
         <v>218</v>
       </c>
+      <c r="I51" s="16">
+        <v>218</v>
+      </c>
+      <c r="J51" s="16">
+        <v>218</v>
+      </c>
+      <c r="K51" s="16">
+        <v>218</v>
+      </c>
+      <c r="L51" s="16">
+        <v>218</v>
+      </c>
+      <c r="M51" s="16">
+        <v>218</v>
+      </c>
     </row>
     <row r="52">
       <c r="B52" s="11" t="inlineStr">
@@ -1523,22 +2351,37 @@
       <c r="D52" s="12">
         <v>0</v>
       </c>
-      <c r="E52" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F52" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G52" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H52" s="12" t="inlineStr">
+      <c r="E52" s="12">
+        <v>0</v>
+      </c>
+      <c r="F52" s="12">
+        <v>0</v>
+      </c>
+      <c r="G52" s="12">
+        <v>0</v>
+      </c>
+      <c r="H52" s="12">
+        <v>0</v>
+      </c>
+      <c r="I52" s="12">
+        <v>0</v>
+      </c>
+      <c r="J52" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K52" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L52" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M52" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1568,6 +2411,21 @@
       <c r="H53" s="16">
         <v>0</v>
       </c>
+      <c r="I53" s="16">
+        <v>0</v>
+      </c>
+      <c r="J53" s="16">
+        <v>0</v>
+      </c>
+      <c r="K53" s="16">
+        <v>0</v>
+      </c>
+      <c r="L53" s="16">
+        <v>0</v>
+      </c>
+      <c r="M53" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="B54" s="11" t="inlineStr">
@@ -1581,22 +2439,37 @@
       <c r="D54" s="12">
         <v>0</v>
       </c>
-      <c r="E54" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F54" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G54" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H54" s="12" t="inlineStr">
+      <c r="E54" s="12">
+        <v>0</v>
+      </c>
+      <c r="F54" s="12">
+        <v>0</v>
+      </c>
+      <c r="G54" s="12">
+        <v>0</v>
+      </c>
+      <c r="H54" s="12">
+        <v>0</v>
+      </c>
+      <c r="I54" s="12">
+        <v>0</v>
+      </c>
+      <c r="J54" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K54" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L54" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M54" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1611,11 +2484,15 @@
       <c r="C55" s="16">
         <v/>
       </c>
-      <c r="D55" s="16">
-        <v>0</v>
-      </c>
-      <c r="E55" s="16">
-        <v>0</v>
+      <c r="D55" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E55" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F55" s="16">
         <v>0</v>
@@ -1624,6 +2501,21 @@
         <v>0</v>
       </c>
       <c r="H55" s="16">
+        <v>0</v>
+      </c>
+      <c r="I55" s="16">
+        <v>0</v>
+      </c>
+      <c r="J55" s="16">
+        <v>0</v>
+      </c>
+      <c r="K55" s="16">
+        <v>0</v>
+      </c>
+      <c r="L55" s="16">
+        <v>0</v>
+      </c>
+      <c r="M55" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1637,18 +2529,33 @@
         <v/>
       </c>
       <c r="D56" s="12">
+        <v>143826</v>
+      </c>
+      <c r="E56" s="12">
+        <v>302333</v>
+      </c>
+      <c r="F56" s="12">
+        <v>291701</v>
+      </c>
+      <c r="G56" s="12">
+        <v>285679</v>
+      </c>
+      <c r="H56" s="12">
+        <v>282398</v>
+      </c>
+      <c r="I56" s="12">
         <v>513421</v>
       </c>
-      <c r="E56" s="12">
+      <c r="J56" s="12">
         <v>812525</v>
       </c>
-      <c r="F56" s="12">
+      <c r="K56" s="12">
         <v>544414</v>
       </c>
-      <c r="G56" s="12">
+      <c r="L56" s="12">
         <v>1331458</v>
       </c>
-      <c r="H56" s="12">
+      <c r="M56" s="12">
         <v>2926898</v>
       </c>
     </row>
@@ -1662,18 +2569,33 @@
         <v/>
       </c>
       <c r="D57" s="18">
+        <v>419044</v>
+      </c>
+      <c r="E57" s="18">
+        <v>577551</v>
+      </c>
+      <c r="F57" s="18">
+        <v>566919</v>
+      </c>
+      <c r="G57" s="18">
+        <v>560897</v>
+      </c>
+      <c r="H57" s="18">
+        <v>557616</v>
+      </c>
+      <c r="I57" s="18">
         <v>788639</v>
       </c>
-      <c r="E57" s="18">
+      <c r="J57" s="18">
         <v>1087743</v>
       </c>
-      <c r="F57" s="18">
+      <c r="K57" s="18">
         <v>819632</v>
       </c>
-      <c r="G57" s="18">
+      <c r="L57" s="18">
         <v>1373318</v>
       </c>
-      <c r="H57" s="18">
+      <c r="M57" s="18">
         <v>9011531</v>
       </c>
     </row>
@@ -1687,18 +2609,33 @@
         <v/>
       </c>
       <c r="D58" s="20">
+        <v>1096453</v>
+      </c>
+      <c r="E58" s="20">
+        <v>1255116</v>
+      </c>
+      <c r="F58" s="20">
+        <v>1327262</v>
+      </c>
+      <c r="G58" s="20">
+        <v>1307649</v>
+      </c>
+      <c r="H58" s="20">
+        <v>1412615</v>
+      </c>
+      <c r="I58" s="20">
         <v>1670253</v>
       </c>
-      <c r="E58" s="20">
+      <c r="J58" s="20">
         <v>2053131</v>
       </c>
-      <c r="F58" s="20">
+      <c r="K58" s="20">
         <v>2269143</v>
       </c>
-      <c r="G58" s="20">
+      <c r="L58" s="20">
         <v>4015482</v>
       </c>
-      <c r="H58" s="20">
+      <c r="M58" s="20">
         <v>12958814</v>
       </c>
     </row>
@@ -1722,6 +2659,21 @@
         <v/>
       </c>
       <c r="H59" s="2">
+        <v/>
+      </c>
+      <c r="I59" s="2">
+        <v/>
+      </c>
+      <c r="J59" s="2">
+        <v/>
+      </c>
+      <c r="K59" s="2">
+        <v/>
+      </c>
+      <c r="L59" s="2">
+        <v/>
+      </c>
+      <c r="M59" s="2">
         <v/>
       </c>
     </row>

</xml_diff>